<commit_message>
added figures for dissertation and updated imputation comparison code
</commit_message>
<xml_diff>
--- a/dissertation/Figures/Results/Classification results.xlsx
+++ b/dissertation/Figures/Results/Classification results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2b0b406bfa6151f/GU/Year 4/FYP/MIMIC-III-ML/dissertation/Figures/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="474" documentId="8_{77572494-1EB1-4617-861F-E852B3DF7F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC987EEC-DB7F-488F-9EA4-D59BB084ACEF}"/>
+  <xr:revisionPtr revIDLastSave="725" documentId="8_{77572494-1EB1-4617-861F-E852B3DF7F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{649E6740-F3FC-4C9C-BF52-9BF5BAD3C810}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{84166D81-A993-46BF-BCAE-8BFDBE001F0E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
   <si>
     <t xml:space="preserve">Recall: </t>
   </si>
@@ -61,186 +61,21 @@
     <t>Metric</t>
   </si>
   <si>
-    <t>mean_imputed</t>
-  </si>
-  <si>
-    <t>itr_imputed</t>
-  </si>
-  <si>
-    <t>knn_imputed</t>
-  </si>
-  <si>
-    <t>mice_imputed</t>
-  </si>
-  <si>
-    <t>midas_imputed</t>
-  </si>
-  <si>
     <t>[mean imputed]</t>
   </si>
   <si>
-    <t>f1_macro: 0.716 (+/- 0.038)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.717 (+/- 0.038)</t>
-  </si>
-  <si>
-    <t>Precision: 0.738 (+/- 0.042)</t>
-  </si>
-  <si>
-    <t>Recall: 0.673 (+/- 0.040)</t>
-  </si>
-  <si>
     <t>[most frequent imputed]</t>
   </si>
   <si>
-    <t>f1_macro: 0.702 (+/- 0.021)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.705 (+/- 0.021)</t>
-  </si>
-  <si>
-    <t>Precision: 0.756 (+/- 0.031)</t>
-  </si>
-  <si>
-    <t>Recall: 0.608 (+/- 0.027)</t>
-  </si>
-  <si>
-    <t>[itr imputed]</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.706 (+/- 0.012)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.707 (+/- 0.011)</t>
-  </si>
-  <si>
-    <t>Precision: 0.739 (+/- 0.015)</t>
-  </si>
-  <si>
-    <t>Recall: 0.643 (+/- 0.030)</t>
-  </si>
-  <si>
     <t>[knn imputed]</t>
   </si>
   <si>
-    <t>f1_macro: 0.686 (+/- 0.023)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.687 (+/- 0.022)</t>
-  </si>
-  <si>
-    <t>Precision: 0.704 (+/- 0.022)</t>
-  </si>
-  <si>
-    <t>Recall: 0.645 (+/- 0.053)</t>
-  </si>
-  <si>
     <t>[mice_imputed]</t>
   </si>
   <si>
-    <t>f1_macro: 0.721 (+/- 0.023)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.721 (+/- 0.023)</t>
-  </si>
-  <si>
-    <t>Precision: 0.740 (+/- 0.027)</t>
-  </si>
-  <si>
-    <t>Recall: 0.682 (+/- 0.029)</t>
-  </si>
-  <si>
     <t>[midas_imputed]</t>
   </si>
   <si>
-    <t>f1_macro: 0.695 (+/- 0.030)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.696 (+/- 0.030)</t>
-  </si>
-  <si>
-    <t>Precision: 0.719 (+/- 0.035)</t>
-  </si>
-  <si>
-    <t>Recall: 0.644 (+/- 0.042)</t>
-  </si>
-  <si>
-    <t>Logistic Regresison</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.783 (+/- 0.020)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.779 (+/- 0.027)</t>
-  </si>
-  <si>
-    <t>Precision: 0.787 (+/- 0.027)</t>
-  </si>
-  <si>
-    <t>Recall: 0.778 (+/- 0.021)</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.782 (+/- 0.023)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.785 (+/- 0.020)</t>
-  </si>
-  <si>
-    <t>Precision: 0.790 (+/- 0.019)</t>
-  </si>
-  <si>
-    <t>Recall: 0.785 (+/- 0.031)</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.781 (+/- 0.024)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.784 (+/- 0.025)</t>
-  </si>
-  <si>
-    <t>Precision: 0.788 (+/- 0.022)</t>
-  </si>
-  <si>
-    <t>Recall: 0.772 (+/- 0.033)</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.772 (+/- 0.032)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.771 (+/- 0.027)</t>
-  </si>
-  <si>
-    <t>Precision: 0.783 (+/- 0.031)</t>
-  </si>
-  <si>
-    <t>Recall: 0.754 (+/- 0.038)</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.777 (+/- 0.020)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.777 (+/- 0.019)</t>
-  </si>
-  <si>
-    <t>Precision: 0.803 (+/- 0.024)</t>
-  </si>
-  <si>
-    <t>Recall: 0.736 (+/- 0.042)</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.755 (+/- 0.013)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.756 (+/- 0.017)</t>
-  </si>
-  <si>
-    <t>Precision: 0.779 (+/- 0.021)</t>
-  </si>
-  <si>
-    <t>Recall: 0.736 (+/- 0.021)</t>
-  </si>
-  <si>
     <t>Random Forest</t>
   </si>
   <si>
@@ -259,84 +94,6 @@
     <t>KNN imputed</t>
   </si>
   <si>
-    <t>[mean imputed] f1_macro: 0.708 (+/- 0.030) Accuracy: 0.709 (+/- 0.030) Precision: 0.730 (+/- 0.034) Recall: 0.663 (+/- 0.043)</t>
-  </si>
-  <si>
-    <t>[midas_imputed] f1_macro: 0.701 (+/- 0.016) Accuracy: 0.702 (+/- 0.016) Precision: 0.712 (+/- 0.014) Recall: 0.678 (+/- 0.037)</t>
-  </si>
-  <si>
-    <t>[mice_imputed] f1_macro: 0.725 (+/- 0.015) Accuracy: 0.726 (+/- 0.015) Precision: 0.750 (+/- 0.022) Recall: 0.678 (+/- 0.020)</t>
-  </si>
-  <si>
-    <t>[knn imputed] f1_macro: 0.682 (+/- 0.022) Accuracy: 0.683 (+/- 0.021) Precision: 0.702 (+/- 0.021) Recall: 0.636 (+/- 0.041)</t>
-  </si>
-  <si>
-    <t>[most frequent imputed] f1_macro: 0.711 (+/- 0.014) Accuracy: 0.713 (+/- 0.014) Precision: 0.754 (+/- 0.025) Recall: 0.635 (+/- 0.034)</t>
-  </si>
-  <si>
-    <t>LG</t>
-  </si>
-  <si>
-    <t>SVM</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.790 (+/- 0.026)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.784 (+/- 0.023)</t>
-  </si>
-  <si>
-    <t>Recall: 0.775 (+/- 0.036)</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.785 (+/- 0.012)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.786 (+/- 0.017)</t>
-  </si>
-  <si>
-    <t>Precision: 0.794 (+/- 0.014)</t>
-  </si>
-  <si>
-    <t>Recall: 0.790 (+/- 0.027)</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.766 (+/- 0.023)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.771 (+/- 0.029)</t>
-  </si>
-  <si>
-    <t>Precision: 0.782 (+/- 0.021)</t>
-  </si>
-  <si>
-    <t>Recall: 0.753 (+/- 0.016)</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.772 (+/- 0.019)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.771 (+/- 0.018)</t>
-  </si>
-  <si>
-    <t>Precision: 0.782 (+/- 0.025)</t>
-  </si>
-  <si>
-    <t>Recall: 0.747 (+/- 0.021)</t>
-  </si>
-  <si>
-    <t>f1_macro: 0.769 (+/- 0.018)</t>
-  </si>
-  <si>
-    <t>Accuracy: 0.768 (+/- 0.010)</t>
-  </si>
-  <si>
-    <t>Precision: 0.776 (+/- 0.015)</t>
-  </si>
-  <si>
-    <t>Recall: 0.775 (+/- 0.026)</t>
-  </si>
-  <si>
     <t xml:space="preserve">f1 macro </t>
   </si>
   <si>
@@ -347,13 +104,157 @@
   </si>
   <si>
     <t xml:space="preserve">Recall </t>
+  </si>
+  <si>
+    <t>1st Fold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd Fold </t>
+  </si>
+  <si>
+    <t>3rd Fold</t>
+  </si>
+  <si>
+    <t>Std</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Confidence Interval</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>0.790 (+/- 0.026)</t>
+  </si>
+  <si>
+    <t>0.784 (+/- 0.023)</t>
+  </si>
+  <si>
+    <t>0.788 (+/- 0.022)</t>
+  </si>
+  <si>
+    <t>0.775 (+/- 0.036)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.785 (+/- 0.012)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.786 (+/- 0.017)</t>
+  </si>
+  <si>
+    <t>0.794 (+/- 0.014)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.790 (+/- 0.027)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.766 (+/- 0.023)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.771 (+/- 0.029)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.782 (+/- 0.021)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.753 (+/- 0.016)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.772 (+/- 0.019)</t>
+  </si>
+  <si>
+    <t>0.771 (+/- 0.018)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.782 (+/- 0.025)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.747 (+/- 0.021)</t>
+  </si>
+  <si>
+    <t>0.769 (+/- 0.018)</t>
+  </si>
+  <si>
+    <t>0.768 (+/- 0.010)</t>
+  </si>
+  <si>
+    <t>0.776 (+/- 0.015)</t>
+  </si>
+  <si>
+    <t>0.775 (+/- 0.026)</t>
+  </si>
+  <si>
+    <t>0.708 (+/- 0.03)</t>
+  </si>
+  <si>
+    <t>0.709 (+/- 0.03)</t>
+  </si>
+  <si>
+    <t>0.73 (+/- 0.034)</t>
+  </si>
+  <si>
+    <t>0.663 (+/- 0.043)</t>
+  </si>
+  <si>
+    <t>0.711 (+/- 0.014)</t>
+  </si>
+  <si>
+    <t>0.713 (+/- 0.014)</t>
+  </si>
+  <si>
+    <t>0.754 (+/- 0.025)</t>
+  </si>
+  <si>
+    <t>0.635 (+/- 0.034)</t>
+  </si>
+  <si>
+    <t>0.682 (+/- 0.022)</t>
+  </si>
+  <si>
+    <t>0.683 +/- 0.021)</t>
+  </si>
+  <si>
+    <t>0.702 (+/- 0.021)</t>
+  </si>
+  <si>
+    <t>0.636 (+/- 0.041)</t>
+  </si>
+  <si>
+    <t>0.725 (+/- 0.015)</t>
+  </si>
+  <si>
+    <t>0.726 (+/- 0.015)</t>
+  </si>
+  <si>
+    <t>0.75 (+/- 0.022)</t>
+  </si>
+  <si>
+    <t>0.678 (+/- 0.02)</t>
+  </si>
+  <si>
+    <t>0.701 (+/- 0.016)</t>
+  </si>
+  <si>
+    <t>0.702 (+/- 0.016)</t>
+  </si>
+  <si>
+    <t>0.712 (+/- 0.014)</t>
+  </si>
+  <si>
+    <t>0.678 (+/- 0.037</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +279,11 @@
       <name val="Gill Sans MT"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <name val="Gill Sans MT"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -399,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -409,6 +315,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,46 +759,46 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="24"/>
                   <c:pt idx="0">
-                    <c:v>3.1E-2</c:v>
+                    <c:v>2.5999999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.5000000000000001E-2</c:v>
+                    <c:v>2.3E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>2.1999999999999999E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3.5999999999999997E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.2E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.7000000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.4E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.7E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.3E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>2.9000000000000001E-2</c:v>
                   </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3.3000000000000002E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>2.1999999999999999E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0.02</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.02</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>3.4000000000000002E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="12">
+                    <c:v>2.1000000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>1.6E-2</c:v>
                   </c:pt>
-                  <c:pt idx="11">
-                    <c:v>1.4E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>1.6E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>3.4000000000000002E-2</c:v>
-                  </c:pt>
                   <c:pt idx="15">
+                    <c:v>1.9E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>1.7999999999999999E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>0.02</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>2.5000000000000001E-2</c:v>
@@ -892,16 +807,16 @@
                     <c:v>2.1000000000000001E-2</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>2.1999999999999999E-2</c:v>
+                    <c:v>1.7999999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>2.1999999999999999E-2</c:v>
+                    <c:v>0.01</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>2.4E-2</c:v>
+                    <c:v>1.4999999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>3.1E-2</c:v>
+                    <c:v>2.5999999999999999E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -913,46 +828,46 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="24"/>
                   <c:pt idx="0">
-                    <c:v>3.1E-2</c:v>
+                    <c:v>2.5999999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.5000000000000001E-2</c:v>
+                    <c:v>2.3E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
+                    <c:v>2.1999999999999999E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3.5999999999999997E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.2E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.7000000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.4E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.7E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.3E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>2.9000000000000001E-2</c:v>
                   </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3.3000000000000002E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>2.1999999999999999E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0.02</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.02</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>3.4000000000000002E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="12">
+                    <c:v>2.1000000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
                     <c:v>1.6E-2</c:v>
                   </c:pt>
-                  <c:pt idx="11">
-                    <c:v>1.4E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>1.6E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>3.4000000000000002E-2</c:v>
-                  </c:pt>
                   <c:pt idx="15">
+                    <c:v>1.9E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
                     <c:v>1.7999999999999999E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>0.02</c:v>
                   </c:pt>
                   <c:pt idx="17">
                     <c:v>2.5000000000000001E-2</c:v>
@@ -961,16 +876,16 @@
                     <c:v>2.1000000000000001E-2</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>2.1999999999999999E-2</c:v>
+                    <c:v>1.7999999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>2.1999999999999999E-2</c:v>
+                    <c:v>0.01</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>2.4E-2</c:v>
+                    <c:v>1.4999999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>3.1E-2</c:v>
+                    <c:v>2.5999999999999999E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1081,64 +996,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.77200000000000002</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77600000000000002</c:v>
+                  <c:v>0.78400000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77700000000000002</c:v>
+                  <c:v>0.78800000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.77200000000000002</c:v>
+                  <c:v>0.77500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.77700000000000002</c:v>
+                  <c:v>0.78500000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.77700000000000002</c:v>
+                  <c:v>0.78600000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.77600000000000002</c:v>
+                  <c:v>0.79400000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.77200000000000002</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.76200000000000001</c:v>
+                  <c:v>0.76600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.77100000000000002</c:v>
+                  <c:v>0.71099999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0.78200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.746</c:v>
+                  <c:v>0.753</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>0.77200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.77100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.78200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.747</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.76900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>0.76800000000000002</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.77400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.73699999999999999</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.76700000000000002</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.76</c:v>
-                </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.76900000000000002</c:v>
+                  <c:v>0.77600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.76400000000000001</c:v>
+                  <c:v>0.77500000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1176,7 +1091,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx2"/>
                     </a:solidFill>
@@ -1186,15 +1101,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t>Imputation</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
                   <a:t> Stratigies</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1400"/>
                   <a:t> </a:t>
                 </a:r>
               </a:p>
@@ -1221,7 +1136,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx2"/>
                   </a:solidFill>
@@ -1314,7 +1229,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB" sz="1400"/>
                   <a:t>Score</a:t>
                 </a:r>
               </a:p>
@@ -2400,6 +2315,444 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$133</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$134:$E$138</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.45566800780100192</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.20297783130184549</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.58403767001795348</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.25238858928247881</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.446131520219468</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$E$134:$E$138</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.45566800780100192</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.20297783130184549</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.58403767001795348</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.25238858928247881</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.446131520219468</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$134:$A$138</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>mean imputed</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>most frequent imputed</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>KNN imputed</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MICE imputed</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MIDAS imputed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$134:$F$138</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>26.696666666666669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.169999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.88</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.673333333333336</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CB4D-40A7-8444-FC1ADBD73D13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1862412464"/>
+        <c:axId val="1862407472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1862412464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Imputation Methods</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1862407472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1862407472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>RMSE</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1862412464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2480,6 +2833,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="207">
   <cs:axisTitle>
@@ -3414,6 +3807,511 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx2"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3459,15 +4357,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1030286</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:colOff>1008305</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>37681</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>353291</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
+      <xdr:colOff>331310</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>37681</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3489,6 +4387,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>752473</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1018762</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>173934</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C37FBE34-76E1-4125-BF88-D87B077D14C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3794,10 +4728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D012BA64-D485-42D5-B452-9D690A97790C}">
-  <dimension ref="A2:V131"/>
+  <dimension ref="A2:V149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="F119" sqref="F119"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88:I129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3820,6 +4754,7 @@
     <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="24.5703125" bestFit="1" customWidth="1"/>
@@ -3828,7 +4763,7 @@
     <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -3842,126 +4777,163 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0.77200000000000002</v>
+        <v>0.79</v>
       </c>
       <c r="D3">
-        <v>3.1E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="V3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.77600000000000002</v>
+        <v>0.78400000000000003</v>
       </c>
       <c r="D4">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.3E-2</v>
+      </c>
+      <c r="V4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.77700000000000002</v>
+        <v>0.78800000000000003</v>
       </c>
       <c r="D5">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="V5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.77200000000000002</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="D6">
-        <v>3.3000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="V6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0.77700000000000002</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="D8">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.2E-2</v>
+      </c>
+      <c r="V8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9">
-        <v>0.77700000000000002</v>
+        <v>0.78600000000000003</v>
       </c>
       <c r="D9">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0.77600000000000002</v>
+        <v>0.79400000000000004</v>
       </c>
       <c r="D10">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.4E-2</v>
+      </c>
+      <c r="V10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0.77200000000000002</v>
+        <v>0.79</v>
       </c>
       <c r="D11">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.7E-2</v>
+      </c>
+      <c r="V11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13">
-        <v>0.76200000000000001</v>
+        <v>0.76600000000000001</v>
       </c>
       <c r="D13">
-        <v>1.6E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.3E-2</v>
+      </c>
+      <c r="V13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14">
-        <v>0.77100000000000002</v>
+        <v>0.71099999999999997</v>
       </c>
       <c r="D14">
-        <v>1.4E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="V14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -3969,136 +4941,191 @@
         <v>0.78200000000000003</v>
       </c>
       <c r="D15">
-        <v>1.6E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0.746</v>
+        <v>0.753</v>
       </c>
       <c r="D16">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.6E-2</v>
+      </c>
+      <c r="V16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="C18">
-        <v>0.76800000000000002</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="D18">
-        <v>1.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.9E-2</v>
+      </c>
+      <c r="V18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19">
-        <v>0.77400000000000002</v>
+        <v>0.77100000000000002</v>
       </c>
       <c r="D19">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="V19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0.8</v>
+        <v>0.78200000000000003</v>
       </c>
       <c r="D20">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="V20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0.73699999999999999</v>
+        <v>0.747</v>
       </c>
       <c r="D21">
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
       <c r="C23">
-        <v>0.76700000000000002</v>
+        <v>0.76900000000000002</v>
       </c>
       <c r="D23">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="V23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>2</v>
       </c>
       <c r="C24">
-        <v>0.76</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="D24">
-        <v>2.1999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+      <c r="V24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="C25">
-        <v>0.76900000000000002</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="D25">
-        <v>2.4E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0.76400000000000001</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="D26">
-        <v>3.1E-2</v>
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="V26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V42" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T43" t="s">
-        <v>43</v>
-      </c>
       <c r="V43" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T44" t="s">
-        <v>13</v>
-      </c>
       <c r="V44" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T45" t="s">
-        <v>14</v>
-      </c>
-      <c r="V45" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.25">
@@ -4114,19 +5141,16 @@
       <c r="D46" t="s">
         <v>5</v>
       </c>
-      <c r="T46" t="s">
-        <v>15</v>
-      </c>
       <c r="V46" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="C47">
         <v>0.70799999999999996</v>
@@ -4134,16 +5158,13 @@
       <c r="D47">
         <v>0.03</v>
       </c>
-      <c r="T47" t="s">
-        <v>16</v>
-      </c>
       <c r="V47" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="C48">
         <v>0.70899999999999996</v>
@@ -4151,16 +5172,13 @@
       <c r="D48">
         <v>0.03</v>
       </c>
-      <c r="T48" t="s">
-        <v>17</v>
-      </c>
       <c r="V48" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="C49">
         <v>0.73</v>
@@ -4168,10 +5186,13 @@
       <c r="D49">
         <v>3.4000000000000002E-2</v>
       </c>
+      <c r="V49" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="C50">
         <v>0.66300000000000003</v>
@@ -4179,27 +5200,18 @@
       <c r="D50">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="T50" t="s">
-        <v>18</v>
-      </c>
-      <c r="V50" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T51" t="s">
-        <v>19</v>
-      </c>
       <c r="V51" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="C52">
         <v>0.71099999999999997</v>
@@ -4207,16 +5219,13 @@
       <c r="D52">
         <v>1.4E-2</v>
       </c>
-      <c r="T52" t="s">
-        <v>20</v>
-      </c>
       <c r="V52" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="C53">
         <v>0.71299999999999997</v>
@@ -4224,16 +5233,13 @@
       <c r="D53">
         <v>1.4E-2</v>
       </c>
-      <c r="T53" t="s">
-        <v>21</v>
-      </c>
       <c r="V53" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="C54">
         <v>0.754</v>
@@ -4241,16 +5247,13 @@
       <c r="D54">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="T54" t="s">
-        <v>22</v>
-      </c>
       <c r="V54" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="C55">
         <v>0.63500000000000001</v>
@@ -4260,19 +5263,16 @@
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T56" t="s">
-        <v>23</v>
-      </c>
       <c r="V56" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="C57">
         <v>0.68200000000000005</v>
@@ -4280,16 +5280,13 @@
       <c r="D57">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="T57" t="s">
-        <v>24</v>
-      </c>
       <c r="V57" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="C58">
         <v>0.68300000000000005</v>
@@ -4297,16 +5294,13 @@
       <c r="D58">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="T58" t="s">
-        <v>25</v>
-      </c>
       <c r="V58" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="C59">
         <v>0.70199999999999996</v>
@@ -4314,16 +5308,13 @@
       <c r="D59">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="T59" t="s">
-        <v>26</v>
-      </c>
       <c r="V59" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="C60">
         <v>0.63600000000000001</v>
@@ -4331,19 +5322,18 @@
       <c r="D60">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="T60" t="s">
-        <v>27</v>
-      </c>
-      <c r="V60" t="s">
-        <v>55</v>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V61" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="C62">
         <v>0.72499999999999998</v>
@@ -4351,16 +5341,13 @@
       <c r="D62">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="T62" t="s">
-        <v>28</v>
-      </c>
       <c r="V62" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="C63">
         <v>0.72599999999999998</v>
@@ -4368,16 +5355,13 @@
       <c r="D63">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="T63" t="s">
-        <v>29</v>
-      </c>
       <c r="V63" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="C64">
         <v>0.75</v>
@@ -4385,16 +5369,13 @@
       <c r="D64">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="T64" t="s">
-        <v>30</v>
-      </c>
       <c r="V64" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="C65">
         <v>0.67800000000000005</v>
@@ -4402,27 +5383,13 @@
       <c r="D65">
         <v>0.02</v>
       </c>
-      <c r="T65" t="s">
-        <v>31</v>
-      </c>
-      <c r="V65" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T66" t="s">
-        <v>32</v>
-      </c>
-      <c r="V66" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="C67">
         <v>0.70099999999999996</v>
@@ -4431,9 +5398,9 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="C68">
         <v>0.70199999999999996</v>
@@ -4441,16 +5408,10 @@
       <c r="D68">
         <v>1.6E-2</v>
       </c>
-      <c r="T68" t="s">
-        <v>33</v>
-      </c>
-      <c r="V68" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="C69">
         <v>0.71199999999999997</v>
@@ -4458,16 +5419,10 @@
       <c r="D69">
         <v>1.4E-2</v>
       </c>
-      <c r="T69" t="s">
-        <v>34</v>
-      </c>
-      <c r="V69" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="C70">
         <v>0.67800000000000005</v>
@@ -4475,246 +5430,26 @@
       <c r="D70">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="T70" t="s">
-        <v>35</v>
-      </c>
-      <c r="V70" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T71" t="s">
-        <v>36</v>
-      </c>
-      <c r="V71" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T72" t="s">
-        <v>37</v>
-      </c>
-      <c r="V72" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T74" t="s">
-        <v>38</v>
-      </c>
-      <c r="V74" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T75" t="s">
-        <v>39</v>
-      </c>
-      <c r="V75" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T76" t="s">
-        <v>40</v>
-      </c>
-      <c r="V76" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T77" t="s">
-        <v>41</v>
-      </c>
-      <c r="V77" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="T78" t="s">
-        <v>42</v>
-      </c>
-      <c r="V78" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>6</v>
-      </c>
-      <c r="B82" t="s">
-        <v>8</v>
-      </c>
-      <c r="C82" t="s">
-        <v>9</v>
-      </c>
-      <c r="D82" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="C83">
-        <v>0.77700000000000002</v>
-      </c>
-      <c r="D83">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="E83">
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="F83">
-        <v>0.76700000000000002</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84">
-        <v>0.77600000000000002</v>
-      </c>
-      <c r="C84">
-        <v>0.77700000000000002</v>
-      </c>
-      <c r="D84">
-        <v>0.77100000000000002</v>
-      </c>
-      <c r="E84">
-        <v>0.77400000000000002</v>
-      </c>
-      <c r="F84">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>1</v>
-      </c>
-      <c r="B85">
-        <v>0.77700000000000002</v>
-      </c>
-      <c r="C85">
-        <v>0.77600000000000002</v>
-      </c>
-      <c r="D85">
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="E85">
-        <v>0.8</v>
-      </c>
-      <c r="F85">
-        <v>0.76900000000000002</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>0</v>
-      </c>
-      <c r="B86">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="C86">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="D86">
-        <v>0.746</v>
-      </c>
-      <c r="E86">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="F86">
-        <v>0.76400000000000001</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O89" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O90" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O91" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O92" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>79</v>
-      </c>
-      <c r="O93" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="O94" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O96" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="O97" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="O98" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O99" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
-      <c r="O100" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -4726,7 +5461,7 @@
       <c r="I101" s="2"/>
       <c r="J101" s="2"/>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -4737,11 +5472,8 @@
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
-      <c r="O102" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -4752,11 +5484,8 @@
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
       <c r="J103" s="2"/>
-      <c r="O103" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -4767,11 +5496,8 @@
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
       <c r="J104" s="2"/>
-      <c r="O104" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -4782,98 +5508,46 @@
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
       <c r="J105" s="2"/>
-      <c r="O105" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O106" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O108" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O109" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O110" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O111" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O112" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O114" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" ht="27.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="115" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
       <c r="F115" s="4"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
-      <c r="O115" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="116" spans="1:15" ht="27.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
       <c r="F116" s="4"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
-      <c r="O116" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="117" spans="1:15" ht="27.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
       <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
-      <c r="O117" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" ht="27.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
       <c r="F118" s="4"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
-      <c r="O118" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="119" spans="1:15" ht="27.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
       <c r="F119" s="4"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
     </row>
-    <row r="128" spans="1:15" ht="27.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -4881,7 +5555,7 @@
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
     </row>
-    <row r="129" spans="1:6" ht="27.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -4889,21 +5563,276 @@
       <c r="E129" s="4"/>
       <c r="F129" s="4"/>
     </row>
-    <row r="130" spans="1:6" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="A130" s="3"/>
-      <c r="B130" s="4"/>
-      <c r="C130" s="4"/>
-      <c r="D130" s="4"/>
-      <c r="E130" s="4"/>
+    <row r="130" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
+      <c r="A130" s="5"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="6"/>
+      <c r="D130" s="6"/>
+      <c r="E130" s="6"/>
       <c r="F130" s="4"/>
     </row>
-    <row r="131" spans="1:6" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="A131" s="3"/>
-      <c r="B131" s="4"/>
-      <c r="C131" s="4"/>
-      <c r="D131" s="4"/>
-      <c r="E131" s="4"/>
+    <row r="131" spans="1:8" ht="27.75" x14ac:dyDescent="0.25">
+      <c r="A131" s="5"/>
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
       <c r="F131" s="4"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="2"/>
+      <c r="B132" s="2"/>
+      <c r="C132" s="2"/>
+      <c r="D132" s="2"/>
+      <c r="E132" s="2"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F133" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B134" s="7">
+        <v>26.54</v>
+      </c>
+      <c r="C134" s="8">
+        <v>27.21</v>
+      </c>
+      <c r="D134" s="8">
+        <v>26.34</v>
+      </c>
+      <c r="E134" s="8">
+        <f>STDEVA(B134:D134)</f>
+        <v>0.45566800780100192</v>
+      </c>
+      <c r="F134" s="9">
+        <f>AVERAGE(B134:D134)</f>
+        <v>26.696666666666669</v>
+      </c>
+      <c r="G134" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H134">
+        <f>G134*(E134/SQRT(3))</f>
+        <v>0.51563689205141761</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B135" s="7">
+        <v>18.95</v>
+      </c>
+      <c r="C135" s="8">
+        <v>19.21</v>
+      </c>
+      <c r="D135" s="9">
+        <v>19.350000000000001</v>
+      </c>
+      <c r="E135" s="8">
+        <f t="shared" ref="E135:E138" si="0">STDEVA(B135:D135)</f>
+        <v>0.20297783130184549</v>
+      </c>
+      <c r="F135" s="9">
+        <f t="shared" ref="F135:F138" si="1">AVERAGE(B135:D135)</f>
+        <v>19.169999999999998</v>
+      </c>
+      <c r="G135" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H135">
+        <f t="shared" ref="H135:H138" si="2">G135*(E135/SQRT(3))</f>
+        <v>0.22969103886162801</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B136" s="7">
+        <v>21.1</v>
+      </c>
+      <c r="C136" s="8">
+        <v>21.34</v>
+      </c>
+      <c r="D136" s="9">
+        <v>22.21</v>
+      </c>
+      <c r="E136" s="8">
+        <f t="shared" si="0"/>
+        <v>0.58403767001795348</v>
+      </c>
+      <c r="F136" s="9">
+        <f t="shared" si="1"/>
+        <v>21.55</v>
+      </c>
+      <c r="G136" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H136">
+        <f t="shared" si="2"/>
+        <v>0.66090083976342462</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B137" s="7">
+        <v>18.16</v>
+      </c>
+      <c r="C137" s="8">
+        <v>17.809999999999999</v>
+      </c>
+      <c r="D137" s="8">
+        <v>17.670000000000002</v>
+      </c>
+      <c r="E137" s="8">
+        <f t="shared" si="0"/>
+        <v>0.25238858928247881</v>
+      </c>
+      <c r="F137" s="9">
+        <f t="shared" si="1"/>
+        <v>17.88</v>
+      </c>
+      <c r="G137" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H137">
+        <f t="shared" si="2"/>
+        <v>0.28560457512675291</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>17</v>
+      </c>
+      <c r="B138" s="7">
+        <v>29.1</v>
+      </c>
+      <c r="C138" s="8">
+        <v>28.21</v>
+      </c>
+      <c r="D138" s="8">
+        <v>28.71</v>
+      </c>
+      <c r="E138" s="8">
+        <f t="shared" si="0"/>
+        <v>0.446131520219468</v>
+      </c>
+      <c r="F138" s="9">
+        <f t="shared" si="1"/>
+        <v>28.673333333333336</v>
+      </c>
+      <c r="G138" s="2">
+        <v>1.96</v>
+      </c>
+      <c r="H138">
+        <f t="shared" si="2"/>
+        <v>0.50484534045366625</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B139" s="2"/>
+      <c r="C139" s="2"/>
+      <c r="E139" s="2"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="2"/>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" s="2"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="2"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
+      <c r="D142" s="2"/>
+      <c r="E142" s="2"/>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
+      <c r="E143" s="2"/>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>27</v>
+      </c>
+      <c r="B144" s="8">
+        <f>AVERAGE(B134:D134)</f>
+        <v>26.696666666666669</v>
+      </c>
+      <c r="C144" s="2"/>
+      <c r="D144" s="2"/>
+      <c r="E144" s="2"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="2"/>
+      <c r="B145" s="2"/>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+      <c r="E145" s="2"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="2"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="2"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="2"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="2"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>